<commit_message>
Update Reporte, Anadiendo cifras de asistencia
</commit_message>
<xml_diff>
--- a/Resultados/Datos/Asistencia.xlsx
+++ b/Resultados/Datos/Asistencia.xlsx
@@ -404,8 +404,10 @@
       <c r="D2">
         <v>29745</v>
       </c>
-      <c r="E2">
-        <v>1</v>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
       </c>
       <c r="F2">
         <v>0.8656621951862726</v>
@@ -426,8 +428,10 @@
       <c r="D3">
         <v>7409</v>
       </c>
-      <c r="E3">
-        <v>0</v>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="F3">
         <v>0.7268592605070328</v>
@@ -448,8 +452,10 @@
       <c r="D4">
         <v>3485</v>
       </c>
-      <c r="E4">
-        <v>1</v>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
       </c>
       <c r="F4">
         <v>0.0934018851756641</v>
@@ -470,8 +476,10 @@
       <c r="D5">
         <v>1495</v>
       </c>
-      <c r="E5">
-        <v>0</v>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="F5">
         <v>0.7576279142544203</v>
@@ -492,8 +500,10 @@
       <c r="D6">
         <v>6329</v>
       </c>
-      <c r="E6">
-        <v>1</v>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
       </c>
       <c r="F6">
         <v>0.4353417216340558</v>
@@ -502,7 +512,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Arekipa</t>
+          <t>Arequipa</t>
         </is>
       </c>
       <c r="B7">
@@ -514,8 +524,10 @@
       <c r="D7">
         <v>279</v>
       </c>
-      <c r="E7">
-        <v>1</v>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
       </c>
       <c r="F7">
         <v>0.3531786074672049</v>
@@ -536,8 +548,10 @@
       <c r="D8">
         <v>83</v>
       </c>
-      <c r="E8">
-        <v>0</v>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="F8">
         <v>0.1895261845386534</v>
@@ -558,8 +572,10 @@
       <c r="D9">
         <v>57</v>
       </c>
-      <c r="E9">
-        <v>0</v>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="F9">
         <v>0.1748942172073343</v>

</xml_diff>